<commit_message>
updated callback to aws api, quicker aurion close down with parallel activity
</commit_message>
<xml_diff>
--- a/Processes/HR_PositionsTransfer/Data/Config.xlsx
+++ b/Processes/HR_PositionsTransfer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Env\projects\UQ\UiPath\RpaUiPathProcess\Processes\HR_PositionsTransfer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F15A348-E361-4B8F-8B0A-8CC94B7B2C95}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70CDAB4-1E7E-4D10-BA1C-1A17B4DDE693}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -153,15 +153,6 @@
     <t>Static part of logging message. Processed Transaction failed with application exception</t>
   </si>
   <si>
-    <t>OrchestratorQueueName</t>
-  </si>
-  <si>
-    <t>KibanaDemoQueue</t>
-  </si>
-  <si>
-    <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
-  </si>
-  <si>
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
@@ -187,13 +178,25 @@
   </si>
   <si>
     <t>Determines whether to get the Credential from Local or Orchestrator.</t>
+  </si>
+  <si>
+    <t>AWS Robot Status API Endpoint URI</t>
+  </si>
+  <si>
+    <t>ApiEndpointUri</t>
+  </si>
+  <si>
+    <t>AuthToken</t>
+  </si>
+  <si>
+    <t>HR_PositionsTransfer_StatusCallbackEndpoint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -204,6 +207,12 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -226,9 +235,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,16 +553,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="42.44140625" customWidth="1"/>
+    <col min="2" max="2" width="79.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.5546875" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
@@ -593,13 +603,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -627,13 +637,13 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -659,29 +669,19 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>43</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" t="s">
-        <v>48</v>
-      </c>
-    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1674,7 +1674,6 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2896,11 +2895,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="65.44140625" customWidth="1"/>
+    <col min="2" max="2" width="39.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2937,8 +2940,22 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3938,5 +3955,6 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated navigation to position
</commit_message>
<xml_diff>
--- a/Processes/HR_PositionsTransfer/Data/Config.xlsx
+++ b/Processes/HR_PositionsTransfer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Env\projects\UQ\UiPath\RpaUiPathProcess\Processes\HR_PositionsTransfer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70CDAB4-1E7E-4D10-BA1C-1A17B4DDE693}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87BD1B6-5D81-4A04-8462-463E3436F529}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4188" yWindow="0" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -178,18 +178,6 @@
   </si>
   <si>
     <t>Determines whether to get the Credential from Local or Orchestrator.</t>
-  </si>
-  <si>
-    <t>AWS Robot Status API Endpoint URI</t>
-  </si>
-  <si>
-    <t>ApiEndpointUri</t>
-  </si>
-  <si>
-    <t>AuthToken</t>
-  </si>
-  <si>
-    <t>HR_PositionsTransfer_StatusCallbackEndpoint</t>
   </si>
 </sst>
 </file>
@@ -2895,9 +2883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2941,21 +2927,9 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>52</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added QueueItem and Transaction logic for new queue items from aws api
</commit_message>
<xml_diff>
--- a/Processes/HR_PositionsTransfer/Data/Config.xlsx
+++ b/Processes/HR_PositionsTransfer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Env\projects\UQ\UiPath\RpaUiPathProcess\Processes\HR_PositionsTransfer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87BD1B6-5D81-4A04-8462-463E3436F529}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84569226-44ED-40EC-8918-E595C1018672}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4188" yWindow="0" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4188" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>Determines whether to get the Credential from Local or Orchestrator.</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>HR_PositionsTransfer</t>
   </si>
 </sst>
 </file>
@@ -541,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -660,16 +666,23 @@
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>43</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>44</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1662,6 +1675,7 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2883,7 +2897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
completed all error handleing with business exceptions and system errors
</commit_message>
<xml_diff>
--- a/Processes/HR_PositionsTransfer/Data/Config.xlsx
+++ b/Processes/HR_PositionsTransfer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Env\projects\UQ\UiPath\RpaUiPathProcess\Processes\HR_PositionsTransfer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84569226-44ED-40EC-8918-E595C1018672}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83D8943-E1E0-4FC7-82BE-B7F0A8CE7023}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4188" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -162,28 +162,55 @@
     <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
   <si>
-    <t>AurionCredential</t>
-  </si>
-  <si>
-    <t>AurionLocal</t>
-  </si>
-  <si>
-    <t>Credentials for the robot to login to Aurion</t>
-  </si>
-  <si>
-    <t>AurionRuntimeEnv</t>
-  </si>
-  <si>
-    <t>Local</t>
-  </si>
-  <si>
-    <t>Determines whether to get the Credential from Local or Orchestrator.</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
     <t>HR_PositionsTransfer</t>
+  </si>
+  <si>
+    <t>AurionRuntimeLocation</t>
+  </si>
+  <si>
+    <t>AurionRuntimeArguements</t>
+  </si>
+  <si>
+    <t>File path to the aurion executable</t>
+  </si>
+  <si>
+    <t>Aurion Executable Arguments that determine the environment</t>
+  </si>
+  <si>
+    <t>M:\aur11_syst\bin\Aurion.exe</t>
+  </si>
+  <si>
+    <t>/adm=M:\Config\AURSYST\ADM /asn=M:\Config\AURSYST\ADM\Aurion.asn /ini=M:\Config\AURSYST\ADM\usys.ini</t>
+  </si>
+  <si>
+    <t>AurionOrchestratorCredentials</t>
+  </si>
+  <si>
+    <t>HR_PositionsTransfer_Aurion_Credentials</t>
+  </si>
+  <si>
+    <t>Aurion Login Credentials</t>
+  </si>
+  <si>
+    <t>HR_PositionsTransfer_BearerToken</t>
+  </si>
+  <si>
+    <t>AuthToken</t>
+  </si>
+  <si>
+    <t>Bearer Token for Authenticating AWS</t>
+  </si>
+  <si>
+    <t>HR_PositionsTransfer_StatusCallbackEndpoint</t>
+  </si>
+  <si>
+    <t>StatusCallbackApiEndpoint</t>
+  </si>
+  <si>
+    <t>AWS Endpoint to Update status of transaction process.</t>
   </si>
 </sst>
 </file>
@@ -232,7 +259,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,17 +574,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
     <col min="2" max="2" width="79.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.5546875" customWidth="1"/>
+    <col min="3" max="3" width="107.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -595,15 +622,15 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -629,12 +656,12 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>51</v>
@@ -663,30 +690,87 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
+      <c r="A5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B10" t="s">
         <v>44</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1676,6 +1760,8 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2895,13 +2981,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="41.77734375" customWidth="1"/>
     <col min="2" max="2" width="39.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="26" width="65.44140625" customWidth="1"/>
   </cols>
@@ -2939,9 +3028,6 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3939,8 +4025,6 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Init for running in test/prod boxes
</commit_message>
<xml_diff>
--- a/Processes/HR_PositionsTransfer/Data/Config.xlsx
+++ b/Processes/HR_PositionsTransfer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Env\projects\UQ\UiPath\RpaUiPathProcess\Processes\HR_PositionsTransfer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83D8943-E1E0-4FC7-82BE-B7F0A8CE7023}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34023DE4-FA99-45F9-853D-696C7D3CDF03}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4188" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -153,6 +153,12 @@
     <t>Static part of logging message. Processed Transaction failed with application exception</t>
   </si>
   <si>
+    <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
+  </si>
+  <si>
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
@@ -162,28 +168,142 @@
     <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
   <si>
-    <t>OrchestratorQueueName</t>
+    <t>OperatingEnvironment</t>
+  </si>
+  <si>
+    <t>Sets Robot to server type: Dev, Test, Staging or Prod</t>
+  </si>
+  <si>
+    <t>UQ_SMTP_SERVER</t>
+  </si>
+  <si>
+    <t>SMTP Server Address</t>
+  </si>
+  <si>
+    <t>UQ_SMTP_PORT</t>
+  </si>
+  <si>
+    <t>SMTP Server Port</t>
+  </si>
+  <si>
+    <t>Shortcut link to start Aurion</t>
+  </si>
+  <si>
+    <t>Email address for task if no PST match found</t>
+  </si>
+  <si>
+    <t>DefaultTaskEmailAddress</t>
+  </si>
+  <si>
+    <t>DevTestEmailAddress</t>
+  </si>
+  <si>
+    <t>SMTP Server Address for dev and test</t>
+  </si>
+  <si>
+    <t>Drive 1 drive letter for Aurion application</t>
+  </si>
+  <si>
+    <t>Drive 2 drive letter for Aurion application</t>
+  </si>
+  <si>
+    <t>Drive 1 file path for Aurion application</t>
+  </si>
+  <si>
+    <t>Drive 2 file path for Aurion application</t>
+  </si>
+  <si>
+    <t>Drive1_DriveLetter-DEV</t>
+  </si>
+  <si>
+    <t>Drive1_FilePath-DEV</t>
+  </si>
+  <si>
+    <t>Drive2_FilePath-DEV</t>
+  </si>
+  <si>
+    <t>AurionLink-DEV</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>\\nas01.storage.uq.edu.au\aurion11_dev</t>
+  </si>
+  <si>
+    <t>Drive2_DriveLetter-DEV</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>\\nas01.storage.uq.edu.au\aur_xtrn</t>
+  </si>
+  <si>
+    <t>Z:\Shortcuts\Aurion 11 AURXTRN urouter.lnk</t>
+  </si>
+  <si>
+    <t>s.debbe@uq.edu.au; s.gururaj@uq.edu.au</t>
+  </si>
+  <si>
+    <t>employeeservices.hr@enquire.uq.edu.au</t>
+  </si>
+  <si>
+    <t>Drive1_DriveLetter-TEST</t>
+  </si>
+  <si>
+    <t>Drive1_FilePath-TEST</t>
+  </si>
+  <si>
+    <t>Drive2_DriveLetter-TEST</t>
+  </si>
+  <si>
+    <t>Drive2_FilePath-TEST</t>
+  </si>
+  <si>
+    <t>AurionLink-TEST</t>
+  </si>
+  <si>
+    <t>Drive1_DriveLetter-STAGING</t>
+  </si>
+  <si>
+    <t>Drive1_FilePath-STAGING</t>
+  </si>
+  <si>
+    <t>Drive2_DriveLetter-STAGING</t>
+  </si>
+  <si>
+    <t>Drive2_FilePath-STAGING</t>
+  </si>
+  <si>
+    <t>AurionLink-STAGING</t>
+  </si>
+  <si>
+    <t>Drive1_DriveLetter-PROD</t>
+  </si>
+  <si>
+    <t>Drive1_FilePath-PROD</t>
+  </si>
+  <si>
+    <t>Drive2_DriveLetter-PROD</t>
+  </si>
+  <si>
+    <t>Drive2_FilePath-PROD</t>
+  </si>
+  <si>
+    <t>AurionLink-PROD</t>
   </si>
   <si>
     <t>HR_PositionsTransfer</t>
   </si>
   <si>
-    <t>AurionRuntimeLocation</t>
-  </si>
-  <si>
-    <t>AurionRuntimeArguements</t>
-  </si>
-  <si>
-    <t>File path to the aurion executable</t>
-  </si>
-  <si>
-    <t>Aurion Executable Arguments that determine the environment</t>
-  </si>
-  <si>
-    <t>M:\aur11_syst\bin\Aurion.exe</t>
-  </si>
-  <si>
-    <t>/adm=M:\Config\AURSYST\ADM /asn=M:\Config\AURSYST\ADM\Aurion.asn /ini=M:\Config\AURSYST\ADM\usys.ini</t>
+    <t>M</t>
+  </si>
+  <si>
+    <t>\\nas01.storage.uq.edu.au\aur11_syst</t>
+  </si>
+  <si>
+    <t>Z:\Shortcuts\Aurion 11 AURSYST urouter.lnk</t>
   </si>
   <si>
     <t>AurionOrchestratorCredentials</t>
@@ -195,19 +315,19 @@
     <t>Aurion Login Credentials</t>
   </si>
   <si>
+    <t>AuthToken</t>
+  </si>
+  <si>
     <t>HR_PositionsTransfer_BearerToken</t>
   </si>
   <si>
-    <t>AuthToken</t>
-  </si>
-  <si>
     <t>Bearer Token for Authenticating AWS</t>
   </si>
   <si>
+    <t>StatusCallbackApiEndpoint</t>
+  </si>
+  <si>
     <t>HR_PositionsTransfer_StatusCallbackEndpoint</t>
-  </si>
-  <si>
-    <t>StatusCallbackApiEndpoint</t>
   </si>
   <si>
     <t>AWS Endpoint to Update status of transaction process.</t>
@@ -217,7 +337,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -228,6 +348,13 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -253,15 +380,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,17 +708,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z974"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="79.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="107.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.109375" customWidth="1"/>
+    <col min="3" max="3" width="68.5546875" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -622,193 +756,299 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-    </row>
-    <row r="4" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
         <v>58</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1735,35 +1975,9 @@
     <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2982,17 +3196,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.77734375" customWidth="1"/>
-    <col min="2" max="2" width="39.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3029,9 +3241,50 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4016,17 +4269,10 @@
     <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C991">
+    <sortCondition ref="B2:B991"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>